<commit_message>
fin écriture fonction sys, pas encore vérifié
</commit_message>
<xml_diff>
--- a/ecoliModel/param_ecoli_2023.xlsx
+++ b/ecoliModel/param_ecoli_2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20397"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Bureau\ecoliModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Emma\Stage_GB5_LBBE\LBBEModelisation\ecoliModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{744104DA-EF10-479D-9CEB-54FD3EAE9E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACDE302-6004-4ECB-9CD3-04C0A094108A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8964" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8964" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="objective" sheetId="1" r:id="rId1"/>
@@ -22,24 +22,11 @@
     <sheet name="kcat" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="321">
   <si>
     <t>ack</t>
   </si>
@@ -56,9 +43,6 @@
     <t>ald</t>
   </si>
   <si>
-    <t>atp-synth</t>
-  </si>
-  <si>
     <t>biomass</t>
   </si>
   <si>
@@ -74,27 +58,6 @@
     <t>edd</t>
   </si>
   <si>
-    <t>ex-ace</t>
-  </si>
-  <si>
-    <t>ex-co2</t>
-  </si>
-  <si>
-    <t>ex-etoh</t>
-  </si>
-  <si>
-    <t>ex-for</t>
-  </si>
-  <si>
-    <t>ex-lac</t>
-  </si>
-  <si>
-    <t>ex-o2</t>
-  </si>
-  <si>
-    <t>ex-suc</t>
-  </si>
-  <si>
     <t>fbp</t>
   </si>
   <si>
@@ -140,12 +103,6 @@
     <t>me</t>
   </si>
   <si>
-    <t>nad-thd</t>
-  </si>
-  <si>
-    <t>nadh-dh</t>
-  </si>
-  <si>
     <t>pdh</t>
   </si>
   <si>
@@ -212,36 +169,9 @@
     <t>zwf</t>
   </si>
   <si>
-    <t>ACETATE-ext</t>
-  </si>
-  <si>
     <t>BIOMASS</t>
   </si>
   <si>
-    <t>CO2-ext</t>
-  </si>
-  <si>
-    <t>ETOH-ext</t>
-  </si>
-  <si>
-    <t>FORMATE-ext</t>
-  </si>
-  <si>
-    <t>GLU-ext</t>
-  </si>
-  <si>
-    <t>H-ext</t>
-  </si>
-  <si>
-    <t>LACTATE-ext</t>
-  </si>
-  <si>
-    <t>OXY-ext</t>
-  </si>
-  <si>
-    <t>SUCC-ext</t>
-  </si>
-  <si>
     <t>km_ack_ACETATE</t>
   </si>
   <si>
@@ -990,12 +920,81 @@
   </si>
   <si>
     <t>km_zwf_NADPH</t>
+  </si>
+  <si>
+    <t>atp_synth</t>
+  </si>
+  <si>
+    <t>ex_ace</t>
+  </si>
+  <si>
+    <t>ex_co2</t>
+  </si>
+  <si>
+    <t>ex_etoh</t>
+  </si>
+  <si>
+    <t>ex_for</t>
+  </si>
+  <si>
+    <t>ex_lac</t>
+  </si>
+  <si>
+    <t>ex_o2</t>
+  </si>
+  <si>
+    <t>ex_suc</t>
+  </si>
+  <si>
+    <t>nad_thd</t>
+  </si>
+  <si>
+    <t>nadh_dh</t>
+  </si>
+  <si>
+    <t>ACETATE_ext</t>
+  </si>
+  <si>
+    <t>CO2_ext</t>
+  </si>
+  <si>
+    <t>ETOH_ext</t>
+  </si>
+  <si>
+    <t>FORMATE_ext</t>
+  </si>
+  <si>
+    <t>GLU_ext</t>
+  </si>
+  <si>
+    <t>H_ext</t>
+  </si>
+  <si>
+    <t>LACTATE_ext</t>
+  </si>
+  <si>
+    <t>SUCC_ext</t>
+  </si>
+  <si>
+    <t>ex_CO2</t>
+  </si>
+  <si>
+    <t>ex_ETOH</t>
+  </si>
+  <si>
+    <t>ex_O2</t>
+  </si>
+  <si>
+    <t>O2_ext</t>
+  </si>
+  <si>
+    <t>na</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.00E+000"/>
@@ -1065,7 +1064,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 4" xfId="1"/>
+    <cellStyle name="Normal 4" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1461,10 +1460,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
@@ -1515,7 +1514,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>298</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1523,7 +1522,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1531,7 +1530,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1539,7 +1538,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1547,7 +1546,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1555,7 +1554,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1563,7 +1562,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>299</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1571,7 +1570,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>300</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -1579,7 +1578,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>301</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -1587,7 +1586,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>302</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1595,7 +1594,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>303</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -1603,7 +1602,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>304</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -1611,7 +1610,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>305</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -1619,7 +1618,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -1627,7 +1626,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -1635,7 +1634,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -1643,7 +1642,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -1651,7 +1650,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -1659,7 +1658,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -1667,7 +1666,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -1675,7 +1674,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -1683,7 +1682,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -1691,7 +1690,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -1699,7 +1698,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -1707,7 +1706,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -1715,7 +1714,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -1723,7 +1722,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -1731,7 +1730,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -1739,7 +1738,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>306</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -1747,7 +1746,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>307</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -1755,7 +1754,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -1763,7 +1762,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -1771,7 +1770,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -1779,7 +1778,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -1787,7 +1786,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -1795,7 +1794,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -1803,7 +1802,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -1811,7 +1810,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -1819,7 +1818,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -1827,7 +1826,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -1835,7 +1834,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -1843,7 +1842,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -1851,7 +1850,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -1859,7 +1858,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -1867,7 +1866,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -1875,7 +1874,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -1883,7 +1882,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -1891,7 +1890,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -1899,7 +1898,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -1907,7 +1906,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -1915,7 +1914,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -1923,7 +1922,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -1941,10 +1940,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
@@ -2001,7 +2000,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>298</v>
       </c>
       <c r="B6" s="2">
         <v>4893</v>
@@ -2010,7 +2009,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>200000</v>
@@ -2019,7 +2018,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="3">
         <v>2562</v>
@@ -2028,7 +2027,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>901</v>
@@ -2037,7 +2036,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <f>3*213</f>
@@ -2047,7 +2046,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>603</v>
@@ -2056,7 +2055,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>299</v>
       </c>
       <c r="B12" s="3">
         <v>188</v>
@@ -2065,7 +2064,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>300</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2074,7 +2073,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>301</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2083,7 +2082,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>302</v>
       </c>
       <c r="B15">
         <v>1425</v>
@@ -2092,7 +2091,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>303</v>
       </c>
       <c r="B16" s="3">
         <v>551</v>
@@ -2101,7 +2100,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>304</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2110,7 +2109,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>305</v>
       </c>
       <c r="B18">
         <v>849</v>
@@ -2119,7 +2118,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B19">
         <f>332*4</f>
@@ -2129,7 +2128,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B20">
         <v>1096</v>
@@ -2138,7 +2137,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B21">
         <v>1868</v>
@@ -2147,7 +2146,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B22">
         <v>1824</v>
@@ -2156,7 +2155,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B23" s="4">
         <v>2682</v>
@@ -2165,7 +2164,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B24">
         <v>331</v>
@@ -2174,7 +2173,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B25" s="4">
         <v>5628</v>
@@ -2183,7 +2182,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B26" s="4">
         <v>7956</v>
@@ -2192,7 +2191,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B27">
         <v>832</v>
@@ -2201,7 +2200,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B28" s="5">
         <v>1736</v>
@@ -2210,7 +2209,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B29">
         <v>21864</v>
@@ -2219,7 +2218,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B30">
         <v>329</v>
@@ -2228,7 +2227,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B31" s="5">
         <v>533</v>
@@ -2237,7 +2236,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B32">
         <v>624</v>
@@ -2246,7 +2245,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B33">
         <v>4500</v>
@@ -2255,7 +2254,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>306</v>
       </c>
       <c r="B34">
         <v>3728</v>
@@ -2264,7 +2263,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>307</v>
       </c>
       <c r="B35" s="2">
         <v>4878</v>
@@ -2273,7 +2272,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B36">
         <v>42096</v>
@@ -2282,7 +2281,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B37">
         <f>320*4</f>
@@ -2292,7 +2291,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B38">
         <f>2*760</f>
@@ -2302,7 +2301,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B39">
         <f>2*468</f>
@@ -2312,7 +2311,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B40">
         <f>432*2</f>
@@ -2322,7 +2321,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B41">
         <v>549</v>
@@ -2331,7 +2330,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B42">
         <v>387</v>
@@ -2340,7 +2339,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B43">
         <v>514</v>
@@ -2349,7 +2348,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B44">
         <v>3532</v>
@@ -2358,7 +2357,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B45">
         <v>540</v>
@@ -2367,7 +2366,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B46">
         <v>1428</v>
@@ -2376,7 +2375,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B47">
         <v>3444</v>
@@ -2385,7 +2384,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B48">
         <f>470*4</f>
@@ -2395,7 +2394,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B49">
         <v>450</v>
@@ -2404,7 +2403,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B50">
         <v>438</v>
@@ -2413,7 +2412,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B51">
         <v>1332</v>
@@ -2422,7 +2421,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B52">
         <v>1068</v>
@@ -2431,7 +2430,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B53">
         <v>634</v>
@@ -2440,7 +2439,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B54">
         <f>255*2</f>
@@ -2449,7 +2448,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B55">
         <f>2*663</f>
@@ -2458,7 +2457,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B56">
         <v>1326</v>
@@ -2466,7 +2465,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B57">
         <v>491</v>
@@ -2484,11 +2483,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2498,7 +2497,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>308</v>
       </c>
       <c r="B1">
         <v>85</v>
@@ -2506,7 +2505,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B2">
         <v>2E-3</v>
@@ -2514,7 +2513,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>309</v>
       </c>
       <c r="B3">
         <v>0.34</v>
@@ -2522,7 +2521,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>310</v>
       </c>
       <c r="B4">
         <v>109</v>
@@ -2530,7 +2529,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>311</v>
       </c>
       <c r="B5" s="2">
         <v>120</v>
@@ -2538,7 +2537,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>312</v>
       </c>
       <c r="B6">
         <v>33</v>
@@ -2546,7 +2545,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>313</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
@@ -2554,7 +2553,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>314</v>
       </c>
       <c r="B8" s="2">
         <v>55</v>
@@ -2562,7 +2561,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>319</v>
       </c>
       <c r="B9" s="6">
         <v>0.21</v>
@@ -2570,7 +2569,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>315</v>
       </c>
       <c r="B10" s="2">
         <v>40</v>
@@ -2588,7 +2587,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B250"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2602,7 +2601,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="B1">
         <v>3.4359883</v>
@@ -2610,7 +2609,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="B2">
         <v>0.15416706999999999</v>
@@ -2618,7 +2617,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="B3">
         <v>0.40208482000000001</v>
@@ -2626,7 +2625,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="B4">
         <v>7.1353680000000003E-2</v>
@@ -2634,7 +2633,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="B5">
         <v>3.4864698000000001</v>
@@ -2642,7 +2641,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="B6">
         <v>2.4203185999999999</v>
@@ -2650,7 +2649,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="B7">
         <v>1.8017316999999999</v>
@@ -2658,7 +2657,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="B8">
         <v>2.4178638000000002E-2</v>
@@ -2666,7 +2665,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="B9">
         <v>7.8602485E-3</v>
@@ -2674,7 +2673,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="B10" s="6">
         <v>1E-3</v>
@@ -2682,7 +2681,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="B11">
         <v>4.1481191000000001E-2</v>
@@ -2690,7 +2689,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="B12">
         <v>0.11298473000000001</v>
@@ -2698,7 +2697,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="B13">
         <v>5.9298483000000006E-2</v>
@@ -2706,7 +2705,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="B14">
         <v>5.4946438999999998</v>
@@ -2714,7 +2713,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="B15" s="6">
         <v>1E-3</v>
@@ -2722,7 +2721,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="B16">
         <v>0.16863838</v>
@@ -2730,7 +2729,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="B17">
         <v>5.9298483000000006E-2</v>
@@ -2738,7 +2737,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="B18">
         <v>7.8151432000000007E-2</v>
@@ -2746,7 +2745,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="B19">
         <v>0.20436478</v>
@@ -2754,7 +2753,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="B20">
         <v>7.8151432000000007E-2</v>
@@ -2762,7 +2761,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="B21" s="7">
         <v>1.3000000000000001E-2</v>
@@ -2770,7 +2769,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="B22">
         <v>0.48</v>
@@ -2778,7 +2777,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="B23" s="6">
         <v>1E-3</v>
@@ -2786,7 +2785,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="B24" s="6">
         <v>1E-3</v>
@@ -2794,7 +2793,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="B25">
         <v>0.55000000000000004</v>
@@ -2802,7 +2801,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="B26">
         <v>0.46201503999999999</v>
@@ -2810,7 +2809,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="B27">
         <v>2.9260067000000001E-2</v>
@@ -2818,7 +2817,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="B28">
         <v>0.35155923</v>
@@ -2826,7 +2825,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="B29">
         <v>0.34176271000000003</v>
@@ -2834,7 +2833,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="B30">
         <v>9.9775582000000002E-2</v>
@@ -2842,7 +2841,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="B31">
         <v>9.955166700000001E-2</v>
@@ -2850,7 +2849,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="B32">
         <v>0.89124067000000007</v>
@@ -2858,7 +2857,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="B33">
         <v>1.4436320000000001E-2</v>
@@ -2866,7 +2865,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="B34">
         <v>0.01</v>
@@ -2874,7 +2873,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="B35">
         <v>0.01</v>
@@ -2882,7 +2881,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="B36">
         <v>4.3098780000000003</v>
@@ -2890,7 +2889,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="B37">
         <v>0.5</v>
@@ -2898,7 +2897,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="B38">
         <v>0.5</v>
@@ -2906,7 +2905,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="B39">
         <v>1.431486</v>
@@ -2914,7 +2913,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="B40">
         <v>9.1276358000000002E-2</v>
@@ -2922,7 +2921,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="B41">
         <v>0.01</v>
@@ -2930,7 +2929,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="B42">
         <v>0.01</v>
@@ -2938,7 +2937,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="B43">
         <v>1.514272E-2</v>
@@ -2946,7 +2945,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="B44">
         <v>6.7236384000000007E-3</v>
@@ -2954,7 +2953,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="B45">
         <v>0.16894701000000001</v>
@@ -2962,7 +2961,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="B46">
         <v>0.1</v>
@@ -2970,7 +2969,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="B47">
         <v>0.31853463999999998</v>
@@ -2978,7 +2977,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="B48">
         <v>0.88058530000000002</v>
@@ -2986,7 +2985,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="B49">
         <v>8.6650189000000002E-2</v>
@@ -2994,7 +2993,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="B50">
         <v>7.5572390000000003E-2</v>
@@ -3002,7 +3001,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="B51">
         <v>7.5572390000000003E-2</v>
@@ -3010,7 +3009,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="B52">
         <v>2.8686021000000003E-2</v>
@@ -3018,7 +3017,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="B53" s="6">
         <v>1E-3</v>
@@ -3026,7 +3025,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="B54" s="6">
         <v>1E-3</v>
@@ -3034,7 +3033,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="B55">
         <v>0.05</v>
@@ -3042,7 +3041,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="B56">
         <v>2E-3</v>
@@ -3050,7 +3049,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="B57">
         <v>2E-3</v>
@@ -3058,7 +3057,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="B58">
         <v>1.4648186000000001E-3</v>
@@ -3066,7 +3065,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="B59">
         <v>0.56077905000000006</v>
@@ -3074,7 +3073,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="B60">
         <v>1.4648186000000001E-3</v>
@@ -3082,7 +3081,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="B61">
         <v>4.3395965000000002E-2</v>
@@ -3090,7 +3089,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="B62">
         <v>0.14959596</v>
@@ -3098,7 +3097,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="B63">
         <v>9.9946203000000011E-2</v>
@@ -3106,7 +3105,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="B64">
         <v>0.10005383</v>
@@ -3114,7 +3113,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="B65" s="6">
         <v>1E-3</v>
@@ -3122,7 +3121,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="B66" s="6">
         <v>1E-3</v>
@@ -3130,7 +3129,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="B67">
         <v>9.9946772000000003E-2</v>
@@ -3138,7 +3137,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="B68">
         <v>0.10005326</v>
@@ -3146,7 +3145,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="B69">
         <v>9.9929218E-2</v>
@@ -3154,7 +3153,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="B70">
         <v>0.10007083</v>
@@ -3162,7 +3161,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="B71">
         <v>9.9938862000000003E-2</v>
@@ -3170,7 +3169,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="B72">
         <v>0.10006118</v>
@@ -3178,7 +3177,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="B73" s="6">
         <v>1E-3</v>
@@ -3186,7 +3185,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="B74" s="6">
         <v>1E-3</v>
@@ -3194,7 +3193,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="B75" s="6">
         <v>1E-3</v>
@@ -3202,7 +3201,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="B76" s="6">
         <v>1E-3</v>
@@ -3210,7 +3209,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="B77">
         <v>9.9963433000000004E-2</v>
@@ -3218,7 +3217,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="B78">
         <v>0.10003658</v>
@@ -3226,7 +3225,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="B79">
         <v>9.9854971000000001E-2</v>
@@ -3234,7 +3233,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="B80">
         <v>0.10014524</v>
@@ -3242,7 +3241,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="B81">
         <v>0.05</v>
@@ -3250,7 +3249,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="B82">
         <v>0.05</v>
@@ -3258,7 +3257,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="B83" s="6">
         <v>1E-3</v>
@@ -3266,7 +3265,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="B84" s="6">
         <v>1E-3</v>
@@ -3274,7 +3273,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="B85">
         <v>9.9985447000000005E-2</v>
@@ -3282,7 +3281,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="B86">
         <v>0.10001456</v>
@@ -3290,7 +3289,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="B87">
         <v>0.170733</v>
@@ -3298,7 +3297,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="B88">
         <v>1.6114823E-2</v>
@@ -3306,7 +3305,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="B89">
         <v>2.0134856E-2</v>
@@ -3314,7 +3313,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="B90">
         <v>4.3142381E-2</v>
@@ -3322,7 +3321,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="B91">
         <v>0.23179063999999999</v>
@@ -3330,7 +3329,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="B92">
         <v>0.20543726000000001</v>
@@ -3338,7 +3337,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="B93">
         <v>0.31389369</v>
@@ -3346,7 +3345,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="B94">
         <v>0.61515012999999996</v>
@@ -3354,7 +3353,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="B95">
         <v>5.7569553000000002E-2</v>
@@ -3362,7 +3361,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="B96">
         <v>0.68673903000000003</v>
@@ -3370,7 +3369,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="B97">
         <v>5.5756399999999998E-2</v>
@@ -3378,7 +3377,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="B98">
         <v>5.7569553000000002E-2</v>
@@ -3386,7 +3385,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="B99" s="2">
         <v>0.125</v>
@@ -3394,7 +3393,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="B100" s="6">
         <v>1E-3</v>
@@ -3402,7 +3401,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="B101" s="2">
         <v>3.97</v>
@@ -3410,7 +3409,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="B102">
         <v>3.7</v>
@@ -3418,7 +3417,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="B103" s="2">
         <v>0.23800000000000002</v>
@@ -3426,7 +3425,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="B104">
         <v>0.16825514</v>
@@ -3434,7 +3433,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="B105">
         <v>5.9433547000000003E-2</v>
@@ -3442,7 +3441,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="B106" s="2">
         <v>2.6000000000000002E-2</v>
@@ -3450,7 +3449,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="B107">
         <v>0.26</v>
@@ -3458,7 +3457,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="B108" s="2">
         <v>3.3</v>
@@ -3466,7 +3465,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="B109" s="2">
         <v>4.9000000000000004</v>
@@ -3474,7 +3473,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="B110">
         <v>0.10300000000000001</v>
@@ -3482,7 +3481,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="B111" s="6">
         <v>1E-3</v>
@@ -3490,7 +3489,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="B112" s="2">
         <v>5.82</v>
@@ -3498,7 +3497,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="B113">
         <v>0.25</v>
@@ -3506,7 +3505,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="B114" s="2">
         <v>1.64</v>
@@ -3514,7 +3513,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="B115" s="2">
         <v>3.7</v>
@@ -3522,7 +3521,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="B116">
         <v>0.48256956000000001</v>
@@ -3530,7 +3529,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="B117">
         <v>2.0223528000000002</v>
@@ -3538,7 +3537,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="B118">
         <v>2.2669351000000001E-2</v>
@@ -3546,7 +3545,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="B119">
         <v>1.0645761</v>
@@ -3554,7 +3553,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="B120">
         <v>1.1912136E-2</v>
@@ -3562,7 +3561,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="B121">
         <v>0.13</v>
@@ -3570,7 +3569,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="B122">
         <v>0.65</v>
@@ -3578,7 +3577,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="B123">
         <v>0.59</v>
@@ -3586,7 +3585,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="B124">
         <v>6.7023310000000003E-2</v>
@@ -3594,7 +3593,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="B125">
         <v>0.10790898</v>
@@ -3602,7 +3601,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="B126">
         <v>9.2670690999999999E-2</v>
@@ -3610,7 +3609,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="B127" s="6">
         <v>1E-3</v>
@@ -3618,7 +3617,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
       <c r="B128">
         <v>9.2670690999999999E-2</v>
@@ -3626,7 +3625,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
       <c r="B129">
         <v>0.10790898</v>
@@ -3634,7 +3633,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
       <c r="B130">
         <v>0.10790898</v>
@@ -3642,7 +3641,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="B131" s="6">
         <v>1E-3</v>
@@ -3650,7 +3649,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
       <c r="B132">
         <v>0.51737429999999995</v>
@@ -3658,7 +3657,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>199</v>
+        <v>180</v>
       </c>
       <c r="B133">
         <v>0.51737436000000003</v>
@@ -3666,7 +3665,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="B134">
         <v>1.9328362000000002E-2</v>
@@ -3674,7 +3673,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>201</v>
+        <v>182</v>
       </c>
       <c r="B135">
         <v>1.9328364000000001E-2</v>
@@ -3682,7 +3681,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>202</v>
+        <v>183</v>
       </c>
       <c r="B136">
         <v>2.1999999999999999E-2</v>
@@ -3690,7 +3689,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>203</v>
+        <v>184</v>
       </c>
       <c r="B137">
         <v>0.05</v>
@@ -3698,7 +3697,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>204</v>
+        <v>185</v>
       </c>
       <c r="B138">
         <v>0.05</v>
@@ -3706,7 +3705,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
       <c r="B139" s="6">
         <v>1E-3</v>
@@ -3714,7 +3713,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
       <c r="B140">
         <v>0.05</v>
@@ -3722,7 +3721,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="B141">
         <v>3.1896955</v>
@@ -3730,7 +3729,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
       <c r="B142">
         <v>0.45965455999999999</v>
@@ -3738,7 +3737,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
       <c r="B143">
         <v>3.2069119E-2</v>
@@ -3746,7 +3745,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>210</v>
+        <v>191</v>
       </c>
       <c r="B144">
         <v>2.8265580000000002E-2</v>
@@ -3754,7 +3753,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>211</v>
+        <v>192</v>
       </c>
       <c r="B145">
         <v>8.8484867000000009E-2</v>
@@ -3762,7 +3761,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>212</v>
+        <v>193</v>
       </c>
       <c r="B146">
         <v>0.36140168</v>
@@ -3770,7 +3769,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>213</v>
+        <v>194</v>
       </c>
       <c r="B147">
         <v>6.9121414000000006E-2</v>
@@ -3778,7 +3777,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="B148">
         <v>8.8484867000000009E-2</v>
@@ -3786,7 +3785,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="B149">
         <v>8.8484867000000009E-2</v>
@@ -3794,7 +3793,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>216</v>
+        <v>197</v>
       </c>
       <c r="B150">
         <v>0.13320000000000001</v>
@@ -3802,7 +3801,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="B151">
         <v>6.3E-2</v>
@@ -3810,7 +3809,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="B152">
         <v>6.3E-2</v>
@@ -3818,7 +3817,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="B153">
         <v>6.8000000000000005E-2</v>
@@ -3826,7 +3825,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
       <c r="B154" s="6">
         <v>1E-3</v>
@@ -3834,7 +3833,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>221</v>
+        <v>202</v>
       </c>
       <c r="B155" s="6">
         <v>1E-3</v>
@@ -3842,7 +3841,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
       <c r="B156">
         <v>5.0000000000000001E-3</v>
@@ -3850,7 +3849,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>223</v>
+        <v>204</v>
       </c>
       <c r="B157" s="3">
         <v>5.0000000000000001E-3</v>
@@ -3858,7 +3857,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
       <c r="B158">
         <v>2E-3</v>
@@ -3866,7 +3865,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>225</v>
+        <v>206</v>
       </c>
       <c r="B159" s="3">
         <v>2E-3</v>
@@ -3874,7 +3873,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>226</v>
+        <v>207</v>
       </c>
       <c r="B160" s="6">
         <v>1E-3</v>
@@ -3882,7 +3881,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="B161" s="6">
         <v>1E-3</v>
@@ -3890,7 +3889,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
       <c r="B162">
         <v>2.8000000000000001E-2</v>
@@ -3898,7 +3897,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
       <c r="B163">
         <v>6.3E-2</v>
@@ -3906,7 +3905,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
       <c r="B164">
         <v>6.3E-2</v>
@@ -3914,7 +3913,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>231</v>
+        <v>212</v>
       </c>
       <c r="B165">
         <v>1.4E-2</v>
@@ -3922,7 +3921,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
       <c r="B166">
         <v>0.15894089</v>
@@ -3930,7 +3929,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
       <c r="B167">
         <v>0.15894089</v>
@@ -3938,7 +3937,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="B168">
         <v>6.2916470000000002E-2</v>
@@ -3946,7 +3945,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>235</v>
+        <v>216</v>
       </c>
       <c r="B169">
         <v>6.2916470000000002E-2</v>
@@ -3954,7 +3953,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>236</v>
+        <v>217</v>
       </c>
       <c r="B170">
         <v>0.15894089</v>
@@ -3962,7 +3961,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>237</v>
+        <v>218</v>
       </c>
       <c r="B171">
         <v>0.29067982000000003</v>
@@ -3970,7 +3969,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="B172">
         <v>0.11341715000000001</v>
@@ -3978,7 +3977,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>239</v>
+        <v>220</v>
       </c>
       <c r="B173">
         <v>0.14095742</v>
@@ -3986,7 +3985,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>240</v>
+        <v>221</v>
       </c>
       <c r="B174">
         <v>0.11627167000000001</v>
@@ -3994,7 +3993,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>241</v>
+        <v>222</v>
       </c>
       <c r="B175">
         <v>0.11341715000000001</v>
@@ -4002,7 +4001,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>242</v>
+        <v>223</v>
       </c>
       <c r="B176">
         <v>3.5199023000000003E-2</v>
@@ -4010,7 +4009,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="B177">
         <v>1.6796243000000002E-2</v>
@@ -4018,7 +4017,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>244</v>
+        <v>225</v>
       </c>
       <c r="B178">
         <v>6.3475273000000003</v>
@@ -4026,7 +4025,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>245</v>
+        <v>226</v>
       </c>
       <c r="B179">
         <v>2.1802383000000001</v>
@@ -4034,7 +4033,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>246</v>
+        <v>227</v>
       </c>
       <c r="B180">
         <v>6.2614572000000007E-2</v>
@@ -4042,7 +4041,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>247</v>
+        <v>228</v>
       </c>
       <c r="B181">
         <v>0.10133236</v>
@@ -4050,7 +4049,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
       <c r="B182">
         <v>5.9104496000000006E-2</v>
@@ -4058,7 +4057,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="B183">
         <v>6.2614572000000007E-2</v>
@@ -4066,7 +4065,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>250</v>
+        <v>231</v>
       </c>
       <c r="B184">
         <v>6.2614572000000007E-2</v>
@@ -4074,7 +4073,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>251</v>
+        <v>232</v>
       </c>
       <c r="B185">
         <v>0.13067264000000001</v>
@@ -4082,7 +4081,7 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>252</v>
+        <v>233</v>
       </c>
       <c r="B186">
         <v>0.10836159999999999</v>
@@ -4090,7 +4089,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
       <c r="B187">
         <v>0.16239803</v>
@@ -4098,7 +4097,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>254</v>
+        <v>235</v>
       </c>
       <c r="B188">
         <v>0.27279660999999999</v>
@@ -4106,7 +4105,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>255</v>
+        <v>236</v>
       </c>
       <c r="B189">
         <v>4.2552917000000003E-2</v>
@@ -4114,7 +4113,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>256</v>
+        <v>237</v>
       </c>
       <c r="B190">
         <v>0.23500151999999999</v>
@@ -4122,7 +4121,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>257</v>
+        <v>238</v>
       </c>
       <c r="B191">
         <v>4.2552917000000003E-2</v>
@@ -4130,7 +4129,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>258</v>
+        <v>239</v>
       </c>
       <c r="B192">
         <v>0.23500151999999999</v>
@@ -4138,7 +4137,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>259</v>
+        <v>240</v>
       </c>
       <c r="B193">
         <v>7.5495268000000004E-2</v>
@@ -4146,7 +4145,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
       <c r="B194">
         <v>0.13245862999999999</v>
@@ -4154,7 +4153,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>261</v>
+        <v>242</v>
       </c>
       <c r="B195">
         <v>0.1145046</v>
@@ -4162,7 +4161,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>262</v>
+        <v>243</v>
       </c>
       <c r="B196" s="6">
         <v>1E-3</v>
@@ -4170,7 +4169,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>263</v>
+        <v>244</v>
       </c>
       <c r="B197">
         <v>4.2589638000000006E-2</v>
@@ -4178,7 +4177,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>264</v>
+        <v>245</v>
       </c>
       <c r="B198">
         <v>0.36370609999999998</v>
@@ -4186,7 +4185,7 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>265</v>
+        <v>246</v>
       </c>
       <c r="B199">
         <v>4.8429688000000005E-2</v>
@@ -4194,7 +4193,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>266</v>
+        <v>247</v>
       </c>
       <c r="B200">
         <v>7.4986177000000001E-2</v>
@@ -4202,7 +4201,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="B201">
         <v>5.2104036999999996</v>
@@ -4210,7 +4209,7 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>268</v>
+        <v>249</v>
       </c>
       <c r="B202">
         <v>0.57097591999999997</v>
@@ -4218,7 +4217,7 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>269</v>
+        <v>250</v>
       </c>
       <c r="B203">
         <v>6.4276432000000008E-2</v>
@@ -4226,7 +4225,7 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>270</v>
+        <v>251</v>
       </c>
       <c r="B204">
         <v>8.7324025E-2</v>
@@ -4234,7 +4233,7 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>271</v>
+        <v>252</v>
       </c>
       <c r="B205">
         <v>3.5012678000000005E-2</v>
@@ -4242,7 +4241,7 @@
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>272</v>
+        <v>253</v>
       </c>
       <c r="B206">
         <v>9.3447325000000012E-2</v>
@@ -4250,7 +4249,7 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>273</v>
+        <v>254</v>
       </c>
       <c r="B207">
         <v>8.641507100000001E-2</v>
@@ -4258,7 +4257,7 @@
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>274</v>
+        <v>255</v>
       </c>
       <c r="B208">
         <v>4.2439428000000001E-2</v>
@@ -4266,7 +4265,7 @@
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>275</v>
+        <v>256</v>
       </c>
       <c r="B209">
         <v>0.31264297000000002</v>
@@ -4274,7 +4273,7 @@
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>276</v>
+        <v>257</v>
       </c>
       <c r="B210">
         <v>8.5984844000000005E-2</v>
@@ -4282,7 +4281,7 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>277</v>
+        <v>258</v>
       </c>
       <c r="B211">
         <v>0.10173498</v>
@@ -4290,7 +4289,7 @@
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>278</v>
+        <v>259</v>
       </c>
       <c r="B212">
         <v>0.11626023000000001</v>
@@ -4298,7 +4297,7 @@
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>279</v>
+        <v>260</v>
       </c>
       <c r="B213">
         <v>9.8294607000000006E-2</v>
@@ -4306,7 +4305,7 @@
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>280</v>
+        <v>261</v>
       </c>
       <c r="B214">
         <v>0.10173498</v>
@@ -4314,7 +4313,7 @@
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
       <c r="B215">
         <v>0.21836598000000002</v>
@@ -4322,7 +4321,7 @@
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>282</v>
+        <v>263</v>
       </c>
       <c r="B216">
         <v>0.35</v>
@@ -4330,7 +4329,7 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>283</v>
+        <v>264</v>
       </c>
       <c r="B217">
         <v>0.2914003</v>
@@ -4338,7 +4337,7 @@
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>284</v>
+        <v>265</v>
       </c>
       <c r="B218">
         <v>4.7641018E-2</v>
@@ -4346,7 +4345,7 @@
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>285</v>
+        <v>266</v>
       </c>
       <c r="B219">
         <v>8.7822018000000002E-2</v>
@@ -4354,7 +4353,7 @@
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="B220">
         <v>0.11386666000000001</v>
@@ -4362,7 +4361,7 @@
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>287</v>
+        <v>268</v>
       </c>
       <c r="B221">
         <v>1.2472893</v>
@@ -4370,7 +4369,7 @@
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>288</v>
+        <v>269</v>
       </c>
       <c r="B222">
         <v>0.55814248</v>
@@ -4378,7 +4377,7 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="B223">
         <v>5.6003086000000001E-2</v>
@@ -4386,7 +4385,7 @@
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>290</v>
+        <v>271</v>
       </c>
       <c r="B224">
         <v>8.1214311000000011E-2</v>
@@ -4394,7 +4393,7 @@
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>291</v>
+        <v>272</v>
       </c>
       <c r="B225">
         <v>7.3087434000000005E-3</v>
@@ -4402,7 +4401,7 @@
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>292</v>
+        <v>273</v>
       </c>
       <c r="B226">
         <v>0.23699996000000001</v>
@@ -4410,7 +4409,7 @@
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>293</v>
+        <v>274</v>
       </c>
       <c r="B227">
         <v>1.0491808E-2</v>
@@ -4418,7 +4417,7 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>294</v>
+        <v>275</v>
       </c>
       <c r="B228">
         <v>8.1233216000000011E-2</v>
@@ -4426,7 +4425,7 @@
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>295</v>
+        <v>276</v>
       </c>
       <c r="B229">
         <v>0.37055218000000001</v>
@@ -4434,7 +4433,7 @@
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>296</v>
+        <v>277</v>
       </c>
       <c r="B230">
         <v>2.6986753000000002E-2</v>
@@ -4442,7 +4441,7 @@
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>297</v>
+        <v>278</v>
       </c>
       <c r="B231">
         <v>0.37055218000000001</v>
@@ -4450,7 +4449,7 @@
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>298</v>
+        <v>279</v>
       </c>
       <c r="B232">
         <v>7.5580976000000008E-2</v>
@@ -4458,7 +4457,7 @@
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>299</v>
+        <v>280</v>
       </c>
       <c r="B233">
         <v>0.17515892</v>
@@ -4466,7 +4465,7 @@
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>300</v>
+        <v>281</v>
       </c>
       <c r="B234">
         <v>0.88809327000000005</v>
@@ -4474,7 +4473,7 @@
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>301</v>
+        <v>282</v>
       </c>
       <c r="B235">
         <v>0.57795788999999997</v>
@@ -4482,7 +4481,7 @@
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>302</v>
+        <v>283</v>
       </c>
       <c r="B236">
         <v>0.20642087000000001</v>
@@ -4490,7 +4489,7 @@
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>303</v>
+        <v>284</v>
       </c>
       <c r="B237">
         <v>7.4991868000000003E-2</v>
@@ -4498,7 +4497,7 @@
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>304</v>
+        <v>285</v>
       </c>
       <c r="B238">
         <v>0.74464775000000005</v>
@@ -4506,7 +4505,7 @@
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>305</v>
+        <v>286</v>
       </c>
       <c r="B239">
         <v>1.2270802000000001</v>
@@ -4514,7 +4513,7 @@
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>306</v>
+        <v>287</v>
       </c>
       <c r="B240">
         <v>0.97227973000000001</v>
@@ -4522,7 +4521,7 @@
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>307</v>
+        <v>288</v>
       </c>
       <c r="B241">
         <v>2.1101234</v>
@@ -4530,7 +4529,7 @@
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>308</v>
+        <v>289</v>
       </c>
       <c r="B242">
         <v>0.1567701</v>
@@ -4538,7 +4537,7 @@
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>309</v>
+        <v>290</v>
       </c>
       <c r="B243">
         <v>9.3367041000000012E-2</v>
@@ -4546,7 +4545,7 @@
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>310</v>
+        <v>291</v>
       </c>
       <c r="B244">
         <v>0.73697349000000001</v>
@@ -4554,7 +4553,7 @@
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>311</v>
+        <v>292</v>
       </c>
       <c r="B245">
         <v>1.2697441999999999</v>
@@ -4562,7 +4561,7 @@
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>312</v>
+        <v>293</v>
       </c>
       <c r="B246">
         <v>0.15150253999999999</v>
@@ -4570,7 +4569,7 @@
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>313</v>
+        <v>294</v>
       </c>
       <c r="B247">
         <v>0.31390635</v>
@@ -4578,7 +4577,7 @@
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>314</v>
+        <v>295</v>
       </c>
       <c r="B248">
         <v>0.12873433000000001</v>
@@ -4586,7 +4585,7 @@
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>315</v>
+        <v>296</v>
       </c>
       <c r="B249">
         <v>0.86322770999999998</v>
@@ -4594,7 +4593,7 @@
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>316</v>
+        <v>297</v>
       </c>
       <c r="B250">
         <v>0.12873433000000001</v>
@@ -4612,11 +4611,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4626,7 +4625,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>316</v>
       </c>
       <c r="B1" s="8">
         <v>4360</v>
@@ -4635,7 +4634,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>317</v>
       </c>
       <c r="B2" s="8">
         <v>2660</v>
@@ -4644,7 +4643,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>318</v>
       </c>
       <c r="B3" s="8">
         <v>4610</v>
@@ -4659,11 +4658,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4714,7 +4713,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>298</v>
       </c>
       <c r="B6" s="6">
         <v>6.2300000000000001E-7</v>
@@ -4722,7 +4721,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>1.0027421000000001</v>
@@ -4730,7 +4729,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="8">
         <v>1200000</v>
@@ -4738,7 +4737,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="6">
         <v>5.9800000000000004E+26</v>
@@ -4746,7 +4745,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="8">
         <v>1.9E-3</v>
@@ -4754,7 +4753,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="8">
         <v>35000000</v>
@@ -4762,7 +4761,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>299</v>
       </c>
       <c r="B12">
         <v>1.0035038999999999</v>
@@ -4770,7 +4769,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>300</v>
       </c>
       <c r="B13">
         <v>1.0034668</v>
@@ -4778,7 +4777,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>301</v>
       </c>
       <c r="B14">
         <v>1.0046131</v>
@@ -4786,7 +4785,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>302</v>
       </c>
       <c r="B15">
         <v>1.0039830999999999</v>
@@ -4794,7 +4793,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>303</v>
       </c>
       <c r="B16">
         <v>1.0023797999999999</v>
@@ -4802,7 +4801,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>304</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -4810,7 +4809,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>305</v>
       </c>
       <c r="B18">
         <v>1.0009465</v>
@@ -4818,7 +4817,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B19">
         <v>101</v>
@@ -4826,7 +4825,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B20" s="8">
         <v>1.7000000000000004E-4</v>
@@ -4834,7 +4833,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B21">
         <v>4.0199999999999996</v>
@@ -4842,7 +4841,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B22">
         <v>4.3300000000000005E-2</v>
@@ -4850,7 +4849,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B23" s="6">
         <v>1.3999999999999999E-6</v>
@@ -4858,7 +4857,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B24" s="8">
         <v>4700</v>
@@ -4866,7 +4865,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B25" s="6">
         <v>480</v>
@@ -4874,7 +4873,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B26" s="6">
         <v>4.2000000000000004E-9</v>
@@ -4883,7 +4882,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B27">
         <v>0.113</v>
@@ -4891,7 +4890,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B28">
         <v>0.02</v>
@@ -4899,7 +4898,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B29" s="8">
         <v>59000</v>
@@ -4907,7 +4906,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B30" s="8">
         <v>65000</v>
@@ -4915,15 +4914,18 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B31" s="9">
         <v>6000000</v>
       </c>
+      <c r="D31" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B32" s="8">
         <v>4.7999999999999998E-6</v>
@@ -4931,7 +4933,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B33" s="8">
         <v>5.2000000000000006E-3</v>
@@ -4939,7 +4941,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>306</v>
       </c>
       <c r="B34" s="3">
         <v>1.49</v>
@@ -4947,7 +4949,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>307</v>
       </c>
       <c r="B35" s="6">
         <v>886000000000</v>
@@ -4955,7 +4957,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B36" s="6">
         <v>1600000</v>
@@ -4963,7 +4965,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B37" s="3">
         <v>420</v>
@@ -4971,7 +4973,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B38" s="8">
         <v>5200</v>
@@ -4979,7 +4981,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B39">
         <v>1.0999999999999999E-2</v>
@@ -4987,7 +4989,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B40">
         <v>5.2</v>
@@ -4995,7 +4997,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B41" s="3">
         <v>0.36099999999999999</v>
@@ -5003,7 +5005,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B42" s="8">
         <v>1700.0000000000002</v>
@@ -5011,7 +5013,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B43">
         <v>0.182</v>
@@ -5019,7 +5021,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B44" s="8">
         <v>2800000</v>
@@ -5027,7 +5029,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B45">
         <v>1.5300000000000001E-2</v>
@@ -5035,7 +5037,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B46">
         <v>1.9E-2</v>
@@ -5043,7 +5045,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B47">
         <v>0.97857957000000007</v>
@@ -5051,7 +5053,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B48" s="8">
         <v>71000</v>
@@ -5060,7 +5062,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B49">
         <v>3.9</v>
@@ -5068,7 +5070,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B50">
         <v>2.1800000000000002</v>
@@ -5076,7 +5078,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B51">
         <v>0.47500000000000003</v>
@@ -5084,7 +5086,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B52" s="6">
         <v>6000</v>
@@ -5092,7 +5094,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B53">
         <v>1.34</v>
@@ -5100,7 +5102,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B54">
         <v>9.1199999999999992</v>
@@ -5108,7 +5110,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B55">
         <v>4.63</v>
@@ -5116,7 +5118,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B56">
         <v>56.3</v>
@@ -5124,7 +5126,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B57">
         <v>2.5499999999999998</v>
@@ -5142,7 +5144,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -5212,7 +5214,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>298</v>
       </c>
       <c r="B6">
         <v>55</v>
@@ -5223,7 +5225,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>99.495737000000005</v>
@@ -5234,7 +5236,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>358.74774000000002</v>
@@ -5245,7 +5247,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="7">
         <v>1461</v>
@@ -5256,7 +5258,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>79.863238999999993</v>
@@ -5267,7 +5269,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>247.49686</v>
@@ -5278,7 +5280,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>299</v>
       </c>
       <c r="B12" s="10">
         <v>100.1</v>
@@ -5289,7 +5291,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>300</v>
       </c>
       <c r="B13">
         <v>100.11987000000001</v>
@@ -5300,7 +5302,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>301</v>
       </c>
       <c r="B14">
         <v>100.15944</v>
@@ -5311,7 +5313,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>302</v>
       </c>
       <c r="B15">
         <v>100.1377</v>
@@ -5322,7 +5324,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>303</v>
       </c>
       <c r="B16">
         <v>100.08231000000001</v>
@@ -5333,7 +5335,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>304</v>
       </c>
       <c r="B17">
         <v>100</v>
@@ -5344,7 +5346,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>305</v>
       </c>
       <c r="B18">
         <v>100.03274999999999</v>
@@ -5355,7 +5357,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B19">
         <v>25.408546999999999</v>
@@ -5366,7 +5368,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B20">
         <v>179.29139000000001</v>
@@ -5377,7 +5379,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B21">
         <v>3380</v>
@@ -5388,7 +5390,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B22">
         <v>233.18129999999999</v>
@@ -5399,7 +5401,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B23">
         <v>13.81</v>
@@ -5410,7 +5412,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B24">
         <v>409.75884000000002</v>
@@ -5421,7 +5423,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B25">
         <v>4.5</v>
@@ -5432,7 +5434,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B26">
         <v>8800</v>
@@ -5443,7 +5445,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B27">
         <v>6727</v>
@@ -5454,7 +5456,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B28">
         <v>3.6</v>
@@ -5465,7 +5467,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B29">
         <v>150.55295000000001</v>
@@ -5476,7 +5478,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B30">
         <v>139.44932</v>
@@ -5487,7 +5489,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B31">
         <v>48.1</v>
@@ -5498,7 +5500,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B32">
         <v>210.74074999999999</v>
@@ -5509,7 +5511,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B33">
         <v>75.937319000000002</v>
@@ -5520,7 +5522,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>306</v>
       </c>
       <c r="B34" s="3">
         <v>259.5</v>
@@ -5531,7 +5533,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>307</v>
       </c>
       <c r="B35" s="7">
         <v>6500</v>
@@ -5542,7 +5544,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B36">
         <v>10895</v>
@@ -5553,7 +5555,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B37">
         <v>1680</v>
@@ -5564,7 +5566,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B38">
         <v>3.8</v>
@@ -5575,7 +5577,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B39">
         <v>110.15501</v>
@@ -5586,7 +5588,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B40">
         <v>210.87804</v>
@@ -5597,7 +5599,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B41">
         <v>321.86315000000002</v>
@@ -5608,7 +5610,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B42">
         <v>390.18351000000001</v>
@@ -5619,7 +5621,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B43">
         <v>1701</v>
@@ -5630,7 +5632,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B44">
         <v>1230.2168200000001</v>
@@ -5641,7 +5643,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B45">
         <v>51.486916999999998</v>
@@ -5652,7 +5654,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B46">
         <v>184146</v>
@@ -5663,7 +5665,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B47">
         <v>103.9461</v>
@@ -5674,7 +5676,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B48">
         <v>513.12070000000006</v>
@@ -5685,7 +5687,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B49">
         <v>133.93446</v>
@@ -5696,7 +5698,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B50">
         <v>1362.0410999999999</v>
@@ -5707,7 +5709,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B51">
         <v>89.247668000000004</v>
@@ -5718,7 +5720,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B52">
         <v>78.129845000000003</v>
@@ -5729,7 +5731,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B53">
         <v>16.742732</v>
@@ -5740,7 +5742,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B54">
         <v>7837.8458000000001</v>
@@ -5751,7 +5753,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B55">
         <v>46.378034999999997</v>
@@ -5762,7 +5764,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B56">
         <v>75.297336000000001</v>
@@ -5773,7 +5775,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B57">
         <v>1486.2</v>

</xml_diff>

<commit_message>
tourne mais errreurs encore sur les noms de variables du excel
</commit_message>
<xml_diff>
--- a/ecoliModel/param_ecoli_2023.xlsx
+++ b/ecoliModel/param_ecoli_2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Emma\Stage_GB5_LBBE\LBBEModelisation\ecoliModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066E7090-523F-4CEE-86E6-C53FF844E055}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA5744E-B86A-4EF0-9C9C-69993396A5B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="7752" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -994,6 +994,9 @@
     <t>km_biomass_P</t>
   </si>
   <si>
+    <t>km_csn_H20</t>
+  </si>
+  <si>
     <t>km_csn_CoA</t>
   </si>
   <si>
@@ -1004,9 +1007,6 @@
   </si>
   <si>
     <t>km_biomass_H2O</t>
-  </si>
-  <si>
-    <t>km_csn_H2O</t>
   </si>
 </sst>
 </file>
@@ -2505,7 +2505,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2819,7 +2819,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B26">
         <v>1E-3</v>
@@ -3027,7 +3027,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B52">
         <v>1E-3</v>
@@ -3051,7 +3051,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B55">
         <v>7.5572390000000003E-2</v>
@@ -3059,7 +3059,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B56">
         <v>1E-3</v>
@@ -3067,7 +3067,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B57">
         <v>1E-3</v>

</xml_diff>

<commit_message>
toujours buf à la multiplication
</commit_message>
<xml_diff>
--- a/ecoliModel/param_ecoli_2023.xlsx
+++ b/ecoliModel/param_ecoli_2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20397"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Emma\Stage_GB5_LBBE\LBBEModelisation\ecoliModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Emma\STAGES_Polytech\Travaux\LBBEModelisation\ecoliModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA5744E-B86A-4EF0-9C9C-69993396A5B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF447E27-4A60-4420-8D48-99DFEAA60F29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="7752" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2295" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="objective" sheetId="1" r:id="rId1"/>
@@ -22,11 +22,24 @@
     <sheet name="kcat" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="340">
   <si>
     <t>ack</t>
   </si>
@@ -367,9 +380,6 @@
     <t>km_kgd_CO2</t>
   </si>
   <si>
-    <t>km_kgd_CoASH</t>
-  </si>
-  <si>
     <t>km_kgd_H</t>
   </si>
   <si>
@@ -436,9 +446,6 @@
     <t>km_pdh_CO2</t>
   </si>
   <si>
-    <t>km_pdh_CoASH</t>
-  </si>
-  <si>
     <t>km_pdh_NAD</t>
   </si>
   <si>
@@ -562,9 +569,6 @@
     <t>km_scs_ATP</t>
   </si>
   <si>
-    <t>km_scs_CoASH</t>
-  </si>
-  <si>
     <t>km_scs_SUCC</t>
   </si>
   <si>
@@ -994,9 +998,6 @@
     <t>km_biomass_P</t>
   </si>
   <si>
-    <t>km_csn_H20</t>
-  </si>
-  <si>
     <t>km_csn_CoA</t>
   </si>
   <si>
@@ -1007,6 +1008,57 @@
   </si>
   <si>
     <t>km_biomass_H2O</t>
+  </si>
+  <si>
+    <t>km_csn_H2O</t>
+  </si>
+  <si>
+    <t>km_gap_P</t>
+  </si>
+  <si>
+    <t>km_gap_H</t>
+  </si>
+  <si>
+    <t>km_gdh_H2O</t>
+  </si>
+  <si>
+    <t>km_kgd_CoA</t>
+  </si>
+  <si>
+    <t>km_mdh_H</t>
+  </si>
+  <si>
+    <t>km_me_NADP</t>
+  </si>
+  <si>
+    <t>km_me_NADPH</t>
+  </si>
+  <si>
+    <t>km_pdh_CoA</t>
+  </si>
+  <si>
+    <t>km_pfk_H</t>
+  </si>
+  <si>
+    <t>km_pyk_H</t>
+  </si>
+  <si>
+    <t>km_scs_P</t>
+  </si>
+  <si>
+    <t>km_zwf_H</t>
+  </si>
+  <si>
+    <t>km_gln_P</t>
+  </si>
+  <si>
+    <t>km_ppc_H2O</t>
+  </si>
+  <si>
+    <t>km_ppc_P</t>
+  </si>
+  <si>
+    <t>km_scs_CoA</t>
   </si>
 </sst>
 </file>
@@ -1058,11 +1110,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1072,13 +1123,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1532,7 +1583,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1580,7 +1631,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1588,7 +1639,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -1596,7 +1647,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -1604,7 +1655,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1612,7 +1663,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -1620,7 +1671,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -1628,7 +1679,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -1756,7 +1807,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -1764,7 +1815,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -2018,9 +2069,9 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>187</v>
-      </c>
-      <c r="B6" s="2">
+        <v>184</v>
+      </c>
+      <c r="B6">
         <v>4893</v>
       </c>
       <c r="D6" s="1"/>
@@ -2038,7 +2089,7 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>2562</v>
       </c>
       <c r="D8" s="1"/>
@@ -2047,7 +2098,7 @@
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9">
         <v>901</v>
       </c>
       <c r="D9" s="1"/>
@@ -2073,16 +2124,16 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>188</v>
-      </c>
-      <c r="B12" s="3">
+        <v>185</v>
+      </c>
+      <c r="B12" s="2">
         <v>188</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2091,7 +2142,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2100,7 +2151,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B15">
         <v>1425</v>
@@ -2109,16 +2160,16 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>192</v>
-      </c>
-      <c r="B16" s="3">
+        <v>189</v>
+      </c>
+      <c r="B16" s="2">
         <v>551</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2127,7 +2178,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B18">
         <v>849</v>
@@ -2175,7 +2226,7 @@
       <c r="A23" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="3">
         <v>2682</v>
       </c>
       <c r="D23" s="1"/>
@@ -2193,7 +2244,7 @@
       <c r="A25" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="3">
         <v>5628</v>
       </c>
       <c r="D25" s="1"/>
@@ -2202,7 +2253,7 @@
       <c r="A26" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="3">
         <v>7956</v>
       </c>
       <c r="D26" s="1"/>
@@ -2220,7 +2271,7 @@
       <c r="A28" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="4">
         <v>1736</v>
       </c>
       <c r="D28" s="1"/>
@@ -2247,7 +2298,7 @@
       <c r="A31" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="4">
         <v>533</v>
       </c>
       <c r="D31" s="1"/>
@@ -2272,7 +2323,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B34">
         <v>3728</v>
@@ -2281,9 +2332,9 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>196</v>
-      </c>
-      <c r="B35" s="2">
+        <v>193</v>
+      </c>
+      <c r="B35">
         <v>4878</v>
       </c>
       <c r="D35" s="1"/>
@@ -2515,7 +2566,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B1">
         <v>85</v>
@@ -2531,7 +2582,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B3">
         <v>0.34</v>
@@ -2539,7 +2590,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B4">
         <v>109</v>
@@ -2547,15 +2598,15 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>200</v>
-      </c>
-      <c r="B5" s="2">
+        <v>197</v>
+      </c>
+      <c r="B5">
         <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B6">
         <v>33</v>
@@ -2563,33 +2614,33 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>202</v>
-      </c>
-      <c r="B7" s="2">
+        <v>199</v>
+      </c>
+      <c r="B7">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>203</v>
-      </c>
-      <c r="B8" s="2">
+        <v>200</v>
+      </c>
+      <c r="B8">
         <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>208</v>
-      </c>
-      <c r="B9" s="6">
+        <v>205</v>
+      </c>
+      <c r="B9" s="5">
         <v>0.21</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>204</v>
-      </c>
-      <c r="B10" s="2">
+        <v>201</v>
+      </c>
+      <c r="B10">
         <v>40</v>
       </c>
     </row>
@@ -2606,10 +2657,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B256"/>
+  <dimension ref="A1:B269"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
+      <selection activeCell="A242" sqref="A242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2627,7 +2678,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B2">
         <v>0.15416706999999999</v>
@@ -2675,7 +2726,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B8">
         <v>2.4178638000000002E-2</v>
@@ -2683,7 +2734,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B9">
         <v>7.8602485E-3</v>
@@ -2691,9 +2742,9 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>317</v>
-      </c>
-      <c r="B10" s="6">
+        <v>314</v>
+      </c>
+      <c r="B10" s="5">
         <v>1E-3</v>
       </c>
     </row>
@@ -2731,9 +2782,9 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>316</v>
-      </c>
-      <c r="B15" s="6">
+        <v>313</v>
+      </c>
+      <c r="B15" s="5">
         <v>1E-3</v>
       </c>
     </row>
@@ -2763,7 +2814,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B19">
         <v>0.20436478</v>
@@ -2771,23 +2822,23 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B20">
         <v>7.8151432000000007E-2</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="B21" s="7">
+      <c r="A21" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="B21" s="6">
         <v>1.3000000000000001E-2</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
-        <v>215</v>
+      <c r="A22" s="6" t="s">
+        <v>212</v>
       </c>
       <c r="B22">
         <v>0.48</v>
@@ -2795,31 +2846,31 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>216</v>
-      </c>
-      <c r="B23" s="6">
+        <v>213</v>
+      </c>
+      <c r="B23" s="5">
         <v>1E-3</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>217</v>
-      </c>
-      <c r="B24" s="6">
+        <v>214</v>
+      </c>
+      <c r="B24" s="5">
         <v>1E-3</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
-        <v>218</v>
+      <c r="A25" s="6" t="s">
+        <v>215</v>
       </c>
       <c r="B25">
         <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="7" t="s">
-        <v>325</v>
+      <c r="A26" s="6" t="s">
+        <v>321</v>
       </c>
       <c r="B26">
         <v>1E-3</v>
@@ -2827,7 +2878,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B27">
         <v>0.46201503999999999</v>
@@ -2875,7 +2926,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B33">
         <v>0.89124067000000007</v>
@@ -2883,7 +2934,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B34">
         <v>1.4436320000000001E-2</v>
@@ -2891,7 +2942,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B35">
         <v>0.01</v>
@@ -2899,7 +2950,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B36">
         <v>0.01</v>
@@ -2907,7 +2958,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B37">
         <v>4.3098780000000003</v>
@@ -2915,7 +2966,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B38">
         <v>0.5</v>
@@ -2923,7 +2974,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B39">
         <v>0.5</v>
@@ -3003,7 +3054,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B49">
         <v>0.88058530000000002</v>
@@ -3011,7 +3062,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B50">
         <v>1E-3</v>
@@ -3019,7 +3070,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B51">
         <v>1E-3</v>
@@ -3027,7 +3078,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B52">
         <v>1E-3</v>
@@ -3035,7 +3086,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B53">
         <v>8.6650189000000002E-2</v>
@@ -3051,7 +3102,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B55">
         <v>7.5572390000000003E-2</v>
@@ -3059,7 +3110,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B56">
         <v>1E-3</v>
@@ -3067,7 +3118,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B57">
         <v>1E-3</v>
@@ -3085,15 +3136,15 @@
       <c r="A59" t="s">
         <v>77</v>
       </c>
-      <c r="B59" s="6">
+      <c r="B59" s="5">
         <v>1E-3</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>228</v>
-      </c>
-      <c r="B60" s="6">
+        <v>225</v>
+      </c>
+      <c r="B60" s="5">
         <v>1E-3</v>
       </c>
     </row>
@@ -3123,7 +3174,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B64">
         <v>1.4648186000000001E-3</v>
@@ -3147,7 +3198,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B67">
         <v>4.3395965000000002E-2</v>
@@ -3163,7 +3214,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B69">
         <v>9.9946203000000011E-2</v>
@@ -3171,7 +3222,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B70">
         <v>0.10005383</v>
@@ -3179,23 +3230,23 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>233</v>
-      </c>
-      <c r="B71" s="6">
+        <v>230</v>
+      </c>
+      <c r="B71" s="5">
         <v>1E-3</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>234</v>
-      </c>
-      <c r="B72" s="6">
+        <v>231</v>
+      </c>
+      <c r="B72" s="5">
         <v>1E-3</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B73">
         <v>9.9946772000000003E-2</v>
@@ -3203,7 +3254,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B74">
         <v>0.10005326</v>
@@ -3211,7 +3262,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B75">
         <v>9.9929218E-2</v>
@@ -3219,7 +3270,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B76">
         <v>0.10007083</v>
@@ -3227,7 +3278,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B77">
         <v>9.9938862000000003E-2</v>
@@ -3235,7 +3286,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B78">
         <v>0.10006118</v>
@@ -3243,39 +3294,39 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>241</v>
-      </c>
-      <c r="B79" s="6">
+        <v>238</v>
+      </c>
+      <c r="B79" s="5">
         <v>1E-3</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>242</v>
-      </c>
-      <c r="B80" s="6">
+        <v>239</v>
+      </c>
+      <c r="B80" s="5">
         <v>1E-3</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>243</v>
-      </c>
-      <c r="B81" s="6">
+        <v>240</v>
+      </c>
+      <c r="B81" s="5">
         <v>1E-3</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>244</v>
-      </c>
-      <c r="B82" s="6">
+        <v>241</v>
+      </c>
+      <c r="B82" s="5">
         <v>1E-3</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B83">
         <v>9.9963433000000004E-2</v>
@@ -3283,7 +3334,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B84">
         <v>0.10003658</v>
@@ -3291,7 +3342,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B85">
         <v>9.9854971000000001E-2</v>
@@ -3299,7 +3350,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B86">
         <v>0.10014524</v>
@@ -3307,7 +3358,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B87">
         <v>0.05</v>
@@ -3315,7 +3366,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B88">
         <v>0.05</v>
@@ -3323,23 +3374,23 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>251</v>
-      </c>
-      <c r="B89" s="6">
+        <v>248</v>
+      </c>
+      <c r="B89" s="5">
         <v>1E-3</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>252</v>
-      </c>
-      <c r="B90" s="6">
+        <v>249</v>
+      </c>
+      <c r="B90" s="5">
         <v>1E-3</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B91">
         <v>9.9985447000000005E-2</v>
@@ -3347,7 +3398,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B92">
         <v>0.10001456</v>
@@ -3355,7 +3406,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B93">
         <v>0.170733</v>
@@ -3363,7 +3414,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B94">
         <v>1.6114823E-2</v>
@@ -3427,271 +3478,271 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>257</v>
+        <v>324</v>
       </c>
       <c r="B102">
-        <v>0.68673903000000003</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>91</v>
+        <v>325</v>
       </c>
       <c r="B103">
-        <v>5.5756399999999998E-2</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
+        <v>254</v>
+      </c>
+      <c r="B104">
+        <v>0.68673903000000003</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>91</v>
+      </c>
+      <c r="B105">
+        <v>5.5756399999999998E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
         <v>92</v>
       </c>
-      <c r="B104">
+      <c r="B106">
         <v>5.7569553000000002E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A105" s="2" t="s">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
         <v>93</v>
       </c>
-      <c r="B105" s="2">
+      <c r="B107">
         <v>0.125</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A106" s="2" t="s">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
         <v>94</v>
       </c>
-      <c r="B106" s="6">
+      <c r="B108" s="5">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A107" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="B107" s="2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>255</v>
+      </c>
+      <c r="B109">
         <v>3.97</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A108" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B108">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A109" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B109" s="2">
-        <v>0.23800000000000002</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>259</v>
+        <v>95</v>
       </c>
       <c r="B110">
-        <v>0.16825514</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>260</v>
+        <v>326</v>
       </c>
       <c r="B111">
-        <v>5.9433547000000003E-2</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A112" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B112" s="2">
-        <v>2.6000000000000002E-2</v>
+      <c r="A112" t="s">
+        <v>96</v>
+      </c>
+      <c r="B112">
+        <v>0.23800000000000002</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
+        <v>256</v>
+      </c>
+      <c r="B113">
+        <v>0.16825514</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>257</v>
+      </c>
+      <c r="B114">
+        <v>5.9433547000000003E-2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>97</v>
+      </c>
+      <c r="B115">
+        <v>2.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
         <v>98</v>
       </c>
-      <c r="B113">
+      <c r="B116">
         <v>0.26</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A114" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="B114" s="2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>336</v>
+      </c>
+      <c r="B117">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>258</v>
+      </c>
+      <c r="B118">
         <v>3.3</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A115" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="B115" s="2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>259</v>
+      </c>
+      <c r="B119">
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A116" s="2" t="s">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
         <v>99</v>
       </c>
-      <c r="B116">
+      <c r="B120">
         <v>0.10300000000000001</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A117" s="2" t="s">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
         <v>100</v>
       </c>
-      <c r="B117" s="6">
+      <c r="B121" s="5">
         <v>1E-3</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A118" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="B118" s="2">
-        <v>5.82</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A119" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="B119">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A120" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B120" s="2">
-        <v>1.64</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A121" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B121" s="2">
-        <v>3.7</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>103</v>
+        <v>260</v>
       </c>
       <c r="B122">
-        <v>0.48256956000000001</v>
+        <v>5.82</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>104</v>
+        <v>261</v>
       </c>
       <c r="B123">
-        <v>2.0223528000000002</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B124">
-        <v>2.2669351000000001E-2</v>
+        <v>1.64</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B125">
-        <v>1.0645761</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B126">
-        <v>1.1912136E-2</v>
+        <v>0.48256956000000001</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B127">
-        <v>0.13</v>
+        <v>2.0223528000000002</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B128">
-        <v>0.65</v>
+        <v>2.2669351000000001E-2</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B129">
-        <v>0.59</v>
+        <v>1.0645761</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B130">
-        <v>6.7023310000000003E-2</v>
+        <v>1.1912136E-2</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B131">
-        <v>0.10790898</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B132">
-        <v>9.2670690999999999E-2</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>114</v>
-      </c>
-      <c r="B133" s="6">
-        <v>1E-3</v>
+        <v>110</v>
+      </c>
+      <c r="B133">
+        <v>0.59</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B134">
-        <v>9.2670690999999999E-2</v>
+        <v>6.7023310000000003E-2</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B135">
         <v>0.10790898</v>
@@ -3699,970 +3750,1074 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>265</v>
+        <v>327</v>
       </c>
       <c r="B136">
-        <v>0.10790898</v>
+        <v>9.2670690999999999E-2</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A137" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B137" s="6">
+      <c r="A137" t="s">
+        <v>113</v>
+      </c>
+      <c r="B137" s="5">
         <v>1E-3</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B138">
-        <v>0.51737429999999995</v>
+        <v>9.2670690999999999E-2</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B139">
-        <v>0.51737436000000003</v>
+        <v>0.10790898</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>120</v>
+        <v>262</v>
       </c>
       <c r="B140">
-        <v>1.9328362000000002E-2</v>
+        <v>0.10790898</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>121</v>
-      </c>
-      <c r="B141">
-        <v>1.9328364000000001E-2</v>
+        <v>116</v>
+      </c>
+      <c r="B141" s="5">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>266</v>
+        <v>117</v>
       </c>
       <c r="B142">
-        <v>2.1999999999999999E-2</v>
+        <v>0.51737429999999995</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B143">
-        <v>0.05</v>
+        <v>0.51737436000000003</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B144">
-        <v>0.05</v>
+        <v>1.9328362000000002E-2</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>124</v>
-      </c>
-      <c r="B145" s="6">
-        <v>1E-3</v>
+        <v>120</v>
+      </c>
+      <c r="B145">
+        <v>1.9328364000000001E-2</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>125</v>
+        <v>263</v>
       </c>
       <c r="B146">
-        <v>0.05</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B147">
-        <v>3.1896955</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B148">
-        <v>0.45965455999999999</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>128</v>
-      </c>
-      <c r="B149">
-        <v>3.2069119E-2</v>
+        <v>123</v>
+      </c>
+      <c r="B149" s="5">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B150">
-        <v>2.8265580000000002E-2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B151">
-        <v>8.8484867000000009E-2</v>
+        <v>3.1896955</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B152">
-        <v>0.36140168</v>
+        <v>0.45965455999999999</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B153">
-        <v>6.9121414000000006E-2</v>
+        <v>3.2069119E-2</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>133</v>
+        <v>328</v>
       </c>
       <c r="B154">
-        <v>8.8484867000000009E-2</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B155">
-        <v>8.8484867000000009E-2</v>
+        <v>2.8265580000000002E-2</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>267</v>
+        <v>129</v>
       </c>
       <c r="B156">
-        <v>0.13320000000000001</v>
+        <v>8.8484867000000009E-2</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>268</v>
+        <v>130</v>
       </c>
       <c r="B157">
-        <v>6.3E-2</v>
+        <v>0.36140168</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>269</v>
+        <v>131</v>
       </c>
       <c r="B158">
-        <v>6.3E-2</v>
+        <v>6.9121414000000006E-2</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>270</v>
+        <v>132</v>
       </c>
       <c r="B159">
-        <v>6.8000000000000005E-2</v>
+        <v>8.8484867000000009E-2</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>271</v>
-      </c>
-      <c r="B160" s="6">
-        <v>1E-3</v>
+        <v>329</v>
+      </c>
+      <c r="B160">
+        <v>6.9120000000000001E-2</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>272</v>
-      </c>
-      <c r="B161" s="6">
-        <v>1E-3</v>
+        <v>330</v>
+      </c>
+      <c r="B161">
+        <v>8.8480000000000003E-2</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>273</v>
+        <v>133</v>
       </c>
       <c r="B162">
-        <v>5.0000000000000001E-3</v>
+        <v>8.8484867000000009E-2</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>274</v>
-      </c>
-      <c r="B163" s="3">
-        <v>5.0000000000000001E-3</v>
+        <v>264</v>
+      </c>
+      <c r="B163">
+        <v>0.13320000000000001</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="B164">
-        <v>2E-3</v>
+        <v>6.3E-2</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>276</v>
-      </c>
-      <c r="B165" s="3">
-        <v>2E-3</v>
+        <v>266</v>
+      </c>
+      <c r="B165">
+        <v>6.3E-2</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>277</v>
-      </c>
-      <c r="B166" s="6">
-        <v>1E-3</v>
+        <v>267</v>
+      </c>
+      <c r="B166">
+        <v>6.8000000000000005E-2</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>278</v>
-      </c>
-      <c r="B167" s="6">
+        <v>268</v>
+      </c>
+      <c r="B167" s="5">
         <v>1E-3</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>279</v>
-      </c>
-      <c r="B168">
-        <v>2.8000000000000001E-2</v>
+        <v>269</v>
+      </c>
+      <c r="B168" s="5">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="B169">
-        <v>6.3E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>281</v>
-      </c>
-      <c r="B170">
-        <v>6.3E-2</v>
+        <v>271</v>
+      </c>
+      <c r="B170" s="2">
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="B171">
-        <v>1.4E-2</v>
+        <v>2E-3</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>283</v>
-      </c>
-      <c r="B172">
-        <v>0.15894089</v>
+        <v>273</v>
+      </c>
+      <c r="B172" s="2">
+        <v>2E-3</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>135</v>
-      </c>
-      <c r="B173">
-        <v>0.15894089</v>
+        <v>274</v>
+      </c>
+      <c r="B173" s="5">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>136</v>
-      </c>
-      <c r="B174">
-        <v>6.2916470000000002E-2</v>
+        <v>275</v>
+      </c>
+      <c r="B174" s="5">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>137</v>
+        <v>276</v>
       </c>
       <c r="B175">
-        <v>6.2916470000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>138</v>
+        <v>277</v>
       </c>
       <c r="B176">
-        <v>0.15894089</v>
+        <v>6.3E-2</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>139</v>
+        <v>278</v>
       </c>
       <c r="B177">
-        <v>0.29067982000000003</v>
+        <v>6.3E-2</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>140</v>
+        <v>279</v>
       </c>
       <c r="B178">
-        <v>0.11341715000000001</v>
+        <v>1.4E-2</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>141</v>
+        <v>280</v>
       </c>
       <c r="B179">
-        <v>0.14095742</v>
+        <v>0.15894089</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>284</v>
+        <v>134</v>
       </c>
       <c r="B180">
-        <v>0.11627167000000001</v>
+        <v>0.15894089</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>285</v>
+        <v>331</v>
       </c>
       <c r="B181">
-        <v>0.11341715000000001</v>
+        <v>6.2916470000000002E-2</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>286</v>
+        <v>135</v>
       </c>
       <c r="B182">
-        <v>3.5199023000000003E-2</v>
+        <v>6.2916470000000002E-2</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B183">
-        <v>1.6796243000000002E-2</v>
+        <v>0.15894089</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B184">
-        <v>6.3475273000000003</v>
+        <v>0.29067982000000003</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B185">
-        <v>2.1802383000000001</v>
+        <v>0.11341715000000001</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B186">
-        <v>6.2614572000000007E-2</v>
+        <v>0.14095742</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="B187">
-        <v>0.10133236</v>
+        <v>0.11627167000000001</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>146</v>
+        <v>332</v>
       </c>
       <c r="B188">
-        <v>5.9104496000000006E-2</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>147</v>
+        <v>282</v>
       </c>
       <c r="B189">
-        <v>6.2614572000000007E-2</v>
+        <v>0.11341715000000001</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B190">
-        <v>6.2614572000000007E-2</v>
+        <v>3.5199023000000003E-2</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B191">
-        <v>0.13067264000000001</v>
+        <v>1.6796243000000002E-2</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B192">
-        <v>0.10836159999999999</v>
+        <v>6.3475273000000003</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>289</v>
+        <v>142</v>
       </c>
       <c r="B193">
-        <v>0.16239803</v>
+        <v>2.1802383000000001</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>290</v>
+        <v>143</v>
       </c>
       <c r="B194">
-        <v>0.27279660999999999</v>
+        <v>6.2614572000000007E-2</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>150</v>
+        <v>284</v>
       </c>
       <c r="B195">
-        <v>4.2552917000000003E-2</v>
+        <v>0.10133236</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B196">
-        <v>0.23500151999999999</v>
+        <v>5.9104496000000006E-2</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B197">
-        <v>4.2552917000000003E-2</v>
+        <v>6.2614572000000007E-2</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>153</v>
+        <v>285</v>
       </c>
       <c r="B198">
-        <v>0.23500151999999999</v>
+        <v>6.2614572000000007E-2</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B199">
-        <v>7.5495268000000004E-2</v>
+        <v>0.13067264000000001</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B200">
-        <v>0.13245862999999999</v>
+        <v>0.10836159999999999</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>156</v>
+        <v>286</v>
       </c>
       <c r="B201">
-        <v>0.1145046</v>
+        <v>0.16239803</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>157</v>
-      </c>
-      <c r="B202" s="6">
-        <v>1E-3</v>
+        <v>287</v>
+      </c>
+      <c r="B202">
+        <v>0.27279660999999999</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="B203">
-        <v>4.2589638000000006E-2</v>
+        <v>4.2552917000000003E-2</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="B204">
-        <v>0.36370609999999998</v>
+        <v>0.23500151999999999</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="B205">
-        <v>4.8429688000000005E-2</v>
+        <v>4.2552917000000003E-2</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="B206">
-        <v>7.4986177000000001E-2</v>
+        <v>0.23500151999999999</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="B207">
-        <v>5.2104036999999996</v>
+        <v>7.5495268000000004E-2</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="B208">
-        <v>0.57097591999999997</v>
+        <v>0.13245862999999999</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="B209">
-        <v>6.4276432000000008E-2</v>
+        <v>0.1145046</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>165</v>
-      </c>
-      <c r="B210">
-        <v>8.7324025E-2</v>
+        <v>155</v>
+      </c>
+      <c r="B210" s="5">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B211">
-        <v>3.5012678000000005E-2</v>
+        <v>4.2589638000000006E-2</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>167</v>
-      </c>
-      <c r="B212">
-        <v>9.3447325000000012E-2</v>
+        <v>337</v>
+      </c>
+      <c r="B212" s="5">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>168</v>
-      </c>
-      <c r="B213">
-        <v>8.641507100000001E-2</v>
+        <v>338</v>
+      </c>
+      <c r="B213" s="5">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>291</v>
+        <v>157</v>
       </c>
       <c r="B214">
-        <v>4.2439428000000001E-2</v>
+        <v>0.36370609999999998</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>292</v>
+        <v>158</v>
       </c>
       <c r="B215">
-        <v>0.31264297000000002</v>
+        <v>4.8429688000000005E-2</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B216">
-        <v>8.5984844000000005E-2</v>
+        <v>7.4986177000000001E-2</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>293</v>
+        <v>160</v>
       </c>
       <c r="B217">
-        <v>0.10173498</v>
+        <v>5.2104036999999996</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>294</v>
+        <v>161</v>
       </c>
       <c r="B218">
-        <v>0.11626023000000001</v>
+        <v>0.57097591999999997</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B219">
-        <v>9.8294607000000006E-2</v>
+        <v>6.4276432000000008E-2</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="B220">
-        <v>0.10173498</v>
+        <v>8.7324025E-2</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="B221">
-        <v>0.21836598000000002</v>
+        <v>3.5012678000000005E-2</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="B222">
-        <v>0.35</v>
+        <v>9.3447325000000012E-2</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="B223">
-        <v>0.2914003</v>
+        <v>8.641507100000001E-2</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>175</v>
+        <v>288</v>
       </c>
       <c r="B224">
-        <v>4.7641018E-2</v>
+        <v>4.2439428000000001E-2</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="B225">
-        <v>8.7822018000000002E-2</v>
+        <v>0.31264297000000002</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>296</v>
+        <v>167</v>
       </c>
       <c r="B226">
-        <v>0.11386666000000001</v>
+        <v>8.5984844000000005E-2</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="B227">
-        <v>1.2472893</v>
+        <v>0.10173498</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="B228">
-        <v>0.55814248</v>
+        <v>0.11626023000000001</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B229">
-        <v>5.6003086000000001E-2</v>
+        <v>9.8294607000000006E-2</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="B230">
-        <v>8.1214311000000011E-2</v>
+        <v>0.10173498</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="B231">
-        <v>7.3087434000000005E-3</v>
+        <v>0.21836598000000002</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="B232">
-        <v>0.23699996000000001</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>299</v>
+        <v>172</v>
       </c>
       <c r="B233">
-        <v>1.0491808E-2</v>
+        <v>0.2914003</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>180</v>
+        <v>333</v>
       </c>
       <c r="B234">
-        <v>8.1233216000000011E-2</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>300</v>
+        <v>173</v>
       </c>
       <c r="B235">
-        <v>0.37055218000000001</v>
+        <v>4.7641018E-2</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>181</v>
+        <v>292</v>
       </c>
       <c r="B236">
-        <v>2.6986753000000002E-2</v>
+        <v>8.7822018000000002E-2</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>182</v>
+        <v>293</v>
       </c>
       <c r="B237">
-        <v>0.37055218000000001</v>
+        <v>0.11386666000000001</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>183</v>
+        <v>294</v>
       </c>
       <c r="B238">
-        <v>7.5580976000000008E-2</v>
+        <v>1.2472893</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="B239">
-        <v>0.17515892</v>
+        <v>0.55814248</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>302</v>
+        <v>174</v>
       </c>
       <c r="B240">
-        <v>0.88809327000000005</v>
+        <v>5.6003086000000001E-2</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>303</v>
+        <v>175</v>
       </c>
       <c r="B241">
-        <v>0.57795788999999997</v>
+        <v>8.1214311000000011E-2</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>304</v>
+        <v>339</v>
       </c>
       <c r="B242">
-        <v>0.20642087000000001</v>
+        <v>7.3087434000000005E-3</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="B243">
-        <v>7.4991868000000003E-2</v>
+        <v>0.23699996000000001</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>305</v>
+        <v>334</v>
       </c>
       <c r="B244">
-        <v>0.74464775000000005</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="B245">
-        <v>1.2270802000000001</v>
+        <v>1.0491808E-2</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>307</v>
+        <v>177</v>
       </c>
       <c r="B246">
-        <v>0.97227973000000001</v>
+        <v>8.1233216000000011E-2</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="B247">
-        <v>2.1101234</v>
+        <v>0.37055218000000001</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>309</v>
+        <v>178</v>
       </c>
       <c r="B248">
-        <v>0.1567701</v>
+        <v>2.6986753000000002E-2</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>310</v>
+        <v>179</v>
       </c>
       <c r="B249">
-        <v>9.3367041000000012E-2</v>
+        <v>0.37055218000000001</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>311</v>
+        <v>180</v>
       </c>
       <c r="B250">
-        <v>0.73697349000000001</v>
+        <v>7.5580976000000008E-2</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
       <c r="B251">
-        <v>1.2697441999999999</v>
+        <v>0.17515892</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
       <c r="B252">
-        <v>0.15150253999999999</v>
+        <v>0.88809327000000005</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="B253">
-        <v>0.31390635</v>
+        <v>0.57795788999999997</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="B254">
-        <v>0.12873433000000001</v>
+        <v>0.20642087000000001</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B255">
-        <v>0.86322770999999998</v>
+        <v>7.4991868000000003E-2</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>186</v>
+        <v>302</v>
       </c>
       <c r="B256">
+        <v>0.74464775000000005</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A257" t="s">
+        <v>303</v>
+      </c>
+      <c r="B257">
+        <v>1.2270802000000001</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A258" t="s">
+        <v>304</v>
+      </c>
+      <c r="B258">
+        <v>0.97227973000000001</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A259" t="s">
+        <v>305</v>
+      </c>
+      <c r="B259">
+        <v>2.1101234</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A260" t="s">
+        <v>306</v>
+      </c>
+      <c r="B260">
+        <v>0.1567701</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A261" t="s">
+        <v>307</v>
+      </c>
+      <c r="B261">
+        <v>9.3367041000000012E-2</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A262" t="s">
+        <v>308</v>
+      </c>
+      <c r="B262">
+        <v>0.73697349000000001</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A263" t="s">
+        <v>309</v>
+      </c>
+      <c r="B263">
+        <v>1.2697441999999999</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A264" t="s">
+        <v>310</v>
+      </c>
+      <c r="B264">
+        <v>0.15150253999999999</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A265" t="s">
+        <v>311</v>
+      </c>
+      <c r="B265">
+        <v>0.31390635</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A266" t="s">
+        <v>312</v>
+      </c>
+      <c r="B266">
         <v>0.12873433000000001</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A267" t="s">
+        <v>182</v>
+      </c>
+      <c r="B267">
+        <v>0.86322770999999998</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A268" t="s">
+        <v>183</v>
+      </c>
+      <c r="B268">
+        <v>0.12873433000000001</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A269" t="s">
+        <v>335</v>
+      </c>
+      <c r="B269">
+        <v>1E-3</v>
       </c>
     </row>
   </sheetData>
@@ -4691,27 +4846,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>205</v>
-      </c>
-      <c r="B1" s="8">
+        <v>202</v>
+      </c>
+      <c r="B1" s="7">
         <v>4360</v>
       </c>
-      <c r="F1" s="8"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>206</v>
-      </c>
-      <c r="B2" s="8">
+        <v>203</v>
+      </c>
+      <c r="B2" s="7">
         <v>2660</v>
       </c>
-      <c r="F2" s="8"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>207</v>
-      </c>
-      <c r="B3" s="8">
+        <v>204</v>
+      </c>
+      <c r="B3" s="7">
         <v>4610</v>
       </c>
     </row>
@@ -4741,7 +4896,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3">
+      <c r="B1" s="2">
         <v>223</v>
       </c>
     </row>
@@ -4757,7 +4912,7 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>1E-3</v>
       </c>
     </row>
@@ -4765,7 +4920,7 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>6300</v>
       </c>
     </row>
@@ -4773,15 +4928,15 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <v>3.4000000000000002E-4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>187</v>
-      </c>
-      <c r="B6" s="6">
+        <v>184</v>
+      </c>
+      <c r="B6" s="5">
         <v>6.2300000000000001E-7</v>
       </c>
     </row>
@@ -4797,7 +4952,7 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="7">
         <v>1200000</v>
       </c>
     </row>
@@ -4805,7 +4960,7 @@
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>5.9800000000000004E+26</v>
       </c>
     </row>
@@ -4813,7 +4968,7 @@
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="7">
         <v>1.9E-3</v>
       </c>
     </row>
@@ -4821,13 +4976,13 @@
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="7">
         <v>35000000</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B12">
         <v>1.0035038999999999</v>
@@ -4835,7 +4990,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B13">
         <v>1.0034668</v>
@@ -4843,7 +4998,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B14">
         <v>1.0046131</v>
@@ -4851,7 +5006,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B15">
         <v>1.0039830999999999</v>
@@ -4859,7 +5014,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B16">
         <v>1.0023797999999999</v>
@@ -4867,7 +5022,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -4875,7 +5030,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B18">
         <v>1.0009465</v>
@@ -4893,7 +5048,7 @@
       <c r="A20" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="7">
         <v>1.7000000000000004E-4</v>
       </c>
     </row>
@@ -4917,7 +5072,7 @@
       <c r="A23" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="5">
         <v>1.3999999999999999E-6</v>
       </c>
     </row>
@@ -4925,7 +5080,7 @@
       <c r="A24" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B24" s="7">
         <v>4700</v>
       </c>
     </row>
@@ -4933,7 +5088,7 @@
       <c r="A25" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="5">
         <v>480</v>
       </c>
     </row>
@@ -4941,10 +5096,10 @@
       <c r="A26" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="5">
         <v>4.2000000000000004E-9</v>
       </c>
-      <c r="D26" s="8"/>
+      <c r="D26" s="7"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -4966,7 +5121,7 @@
       <c r="A29" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="8">
+      <c r="B29" s="7">
         <v>59000</v>
       </c>
     </row>
@@ -4974,7 +5129,7 @@
       <c r="A30" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="8">
+      <c r="B30" s="7">
         <v>65000</v>
       </c>
     </row>
@@ -4982,18 +5137,18 @@
       <c r="A31" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="9">
+      <c r="B31" s="8">
         <v>6000000</v>
       </c>
       <c r="D31" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="8">
+      <c r="B32" s="7">
         <v>4.7999999999999998E-6</v>
       </c>
     </row>
@@ -5001,23 +5156,23 @@
       <c r="A33" t="s">
         <v>24</v>
       </c>
-      <c r="B33" s="8">
+      <c r="B33" s="7">
         <v>5.2000000000000006E-3</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>195</v>
-      </c>
-      <c r="B34" s="3">
+        <v>192</v>
+      </c>
+      <c r="B34" s="2">
         <v>1.49</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>196</v>
-      </c>
-      <c r="B35" s="6">
+        <v>193</v>
+      </c>
+      <c r="B35" s="5">
         <v>886000000000</v>
       </c>
     </row>
@@ -5025,7 +5180,7 @@
       <c r="A36" t="s">
         <v>25</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="5">
         <v>1600000</v>
       </c>
     </row>
@@ -5033,7 +5188,7 @@
       <c r="A37" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="2">
         <v>420</v>
       </c>
     </row>
@@ -5041,7 +5196,7 @@
       <c r="A38" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="8">
+      <c r="B38" s="7">
         <v>5200</v>
       </c>
     </row>
@@ -5065,7 +5220,7 @@
       <c r="A41" t="s">
         <v>30</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41" s="2">
         <v>0.36099999999999999</v>
       </c>
     </row>
@@ -5073,7 +5228,7 @@
       <c r="A42" t="s">
         <v>31</v>
       </c>
-      <c r="B42" s="8">
+      <c r="B42" s="7">
         <v>1700.0000000000002</v>
       </c>
     </row>
@@ -5089,7 +5244,7 @@
       <c r="A44" t="s">
         <v>33</v>
       </c>
-      <c r="B44" s="8">
+      <c r="B44" s="7">
         <v>2800000</v>
       </c>
     </row>
@@ -5121,10 +5276,10 @@
       <c r="A48" t="s">
         <v>37</v>
       </c>
-      <c r="B48" s="8">
+      <c r="B48" s="7">
         <v>71000</v>
       </c>
-      <c r="D48" s="6"/>
+      <c r="D48" s="5"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
@@ -5154,7 +5309,7 @@
       <c r="A52" t="s">
         <v>41</v>
       </c>
-      <c r="B52" s="6">
+      <c r="B52" s="5">
         <v>6000</v>
       </c>
     </row>
@@ -5280,7 +5435,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B6">
         <v>55</v>
@@ -5315,10 +5470,10 @@
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>1461</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>782.98929999999996</v>
       </c>
     </row>
@@ -5346,9 +5501,9 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>188</v>
-      </c>
-      <c r="B12" s="10">
+        <v>185</v>
+      </c>
+      <c r="B12" s="9">
         <v>100.1</v>
       </c>
       <c r="C12">
@@ -5357,7 +5512,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B13">
         <v>100.11987000000001</v>
@@ -5368,7 +5523,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B14">
         <v>100.15944</v>
@@ -5379,7 +5534,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B15">
         <v>100.1377</v>
@@ -5390,7 +5545,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B16">
         <v>100.08231000000001</v>
@@ -5401,7 +5556,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B17">
         <v>100</v>
@@ -5412,7 +5567,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B18">
         <v>100.03274999999999</v>
@@ -5466,7 +5621,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B23">
@@ -5488,7 +5643,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B25">
@@ -5499,7 +5654,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B26">
@@ -5588,9 +5743,9 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>195</v>
-      </c>
-      <c r="B34" s="3">
+        <v>192</v>
+      </c>
+      <c r="B34" s="2">
         <v>259.5</v>
       </c>
       <c r="C34">
@@ -5599,12 +5754,12 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>196</v>
-      </c>
-      <c r="B35" s="7">
+        <v>193</v>
+      </c>
+      <c r="B35" s="6">
         <v>6500</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="6">
         <v>400</v>
       </c>
     </row>

</xml_diff>